<commit_message>
change design form hazop
</commit_message>
<xml_diff>
--- a/dotnet6-epha-api/wwwroot/AttachedFileTemp/HAZOP Report Template-Def.xlsx
+++ b/dotnet6-epha-api/wwwroot/AttachedFileTemp/HAZOP Report Template-Def.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dotnet6-epha-api\dotnet6-epha-api\wwwroot\AttachedFileTemp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A7FF2B-E44F-434D-857E-2FC254CD3D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC1C6FB-1276-48F6-AF78-28493EBF3B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="957" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="957" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HAZOP Cover Page" sheetId="41" r:id="rId1"/>
@@ -18,33 +18,42 @@
     <sheet name="AttendeeSheetTemplate" sheetId="40" r:id="rId3"/>
     <sheet name="Drawing &amp; Reference" sheetId="44" r:id="rId4"/>
     <sheet name="Node List" sheetId="45" r:id="rId5"/>
-    <sheet name="Major Accident Event (MAE)" sheetId="46" r:id="rId6"/>
-    <sheet name="TrackTemplate" sheetId="32" r:id="rId7"/>
-    <sheet name="RecommTemplate" sheetId="37" r:id="rId8"/>
+    <sheet name="TrackTemplate" sheetId="32" r:id="rId6"/>
+    <sheet name="Major Accident Event (MAE)" sheetId="46" r:id="rId7"/>
+    <sheet name="Safety Critical Equipment" sheetId="48" r:id="rId8"/>
     <sheet name="WorksheetTemplate" sheetId="36" r:id="rId9"/>
-    <sheet name="GuidewordsTemplate" sheetId="38" r:id="rId10"/>
-    <sheet name="SheetTemplate" sheetId="39" r:id="rId11"/>
+    <sheet name="Appendix" sheetId="49" r:id="rId10"/>
+    <sheet name="Risk Assessment Matrix" sheetId="39" r:id="rId11"/>
+    <sheet name="GuidewordsTemplate" sheetId="38" r:id="rId12"/>
+    <sheet name="RecommTemplate" sheetId="37" r:id="rId13"/>
+    <sheet name="Drawing PIDs &amp; PFDs" sheetId="50" r:id="rId14"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">Appendix!$A$1:$L$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">AttendeeSheetTemplate!$A$1:$O$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Drawing &amp; Reference'!$A$1:$E$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">GuidewordsTemplate!$A$1:$D$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="13">'Drawing PIDs &amp; PFDs'!$A$1:$J$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">GuidewordsTemplate!$A$1:$D$3</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'HAZOP Cover Page'!$A$1:$L$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Major Accident Event (MAE)'!$A$1:$H$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Major Accident Event (MAE)'!$A$1:$D$3</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Node List'!$A$1:$H$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">RecommTemplate!$A$1:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="12">RecommTemplate!$A$1:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'Risk Assessment Matrix'!$A$1:$J$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Safety Critical Equipment'!$A$1:$O$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Study Objective and Work Scope'!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">TrackTemplate!$A$1:$F$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">TrackTemplate!$A$1:$F$3</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">WorksheetTemplate!$A$1:$P$14</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="9">Appendix!$1:$10</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">AttendeeSheetTemplate!$1:$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Drawing &amp; Reference'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="9">GuidewordsTemplate!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="11">GuidewordsTemplate!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'HAZOP Cover Page'!$1:$17</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Major Accident Event (MAE)'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'Major Accident Event (MAE)'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Node List'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">RecommTemplate!$1:$10</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="12">RecommTemplate!$1:$10</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'Safety Critical Equipment'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Study Objective and Work Scope'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">TrackTemplate!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">TrackTemplate!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">WorksheetTemplate!$1:$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -57,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
   <si>
     <t>RECCOMENDATION STATUS TRACKING TABLE</t>
   </si>
@@ -249,9 +258,6 @@
     <t>Area of Application</t>
   </si>
   <si>
-    <t>HAZOP ATTENDEE SHEET &amp; HAZOP COVER PAGE</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
@@ -404,6 +410,30 @@
   </si>
   <si>
     <t>Major Accident Event (MAE)</t>
+  </si>
+  <si>
+    <t>Risk Asseessment Matrix (R)</t>
+  </si>
+  <si>
+    <t>รายชื่อผู้เข้าร่วม (Attendee list)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety Critical Equipment (SCE) </t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>ตารางการประเมินความเสี่ยง ( Risk Assessment Matrix (RAM) )</t>
+  </si>
+  <si>
+    <t>ภาคผนวก - PIDs / PFDs</t>
+  </si>
+  <si>
+    <t>ภาคผนวก ก
+ข้อมูลและตารางอ้างอิงสําหรับการประเมินความเสี่ยง 
+APPENDIX A 
+PHA -WORKSHEETS</t>
   </si>
 </sst>
 </file>
@@ -933,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -960,24 +990,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1105,6 +1117,52 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1189,6 +1247,15 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1213,6 +1280,135 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1275,141 +1471,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1871,294 +1932,294 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="39" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" style="39" customWidth="1"/>
-    <col min="3" max="6" width="16.33203125" style="39" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" style="57" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" style="57" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" style="57" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="39" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="39" customWidth="1"/>
-    <col min="12" max="12" width="1.77734375" style="39" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="39" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="39"/>
+    <col min="1" max="1" width="5" style="33" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="33" customWidth="1"/>
+    <col min="3" max="6" width="16.33203125" style="33" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="51" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" style="51" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="51" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="33" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="33" customWidth="1"/>
+    <col min="12" max="12" width="1.77734375" style="33" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="33" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="80" t="s">
+      <c r="A1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="37"/>
-    </row>
-    <row r="2" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="80" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="31"/>
+    </row>
+    <row r="3" spans="1:12" ht="179.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+    </row>
+    <row r="4" spans="1:12" ht="310.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="37"/>
-    </row>
-    <row r="3" spans="1:12" ht="179.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-    </row>
-    <row r="4" spans="1:12" ht="310.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="82" t="s">
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" ht="133.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+    </row>
+    <row r="6" spans="1:12" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-    </row>
-    <row r="5" spans="1:12" ht="133.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-    </row>
-    <row r="6" spans="1:12" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="77" t="s">
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="31"/>
+    </row>
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="8" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="37"/>
-    </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-    </row>
-    <row r="8" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="59" t="s">
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="31"/>
+    </row>
+    <row r="9" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="31"/>
+    </row>
+    <row r="12" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="37"/>
-    </row>
-    <row r="9" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="37"/>
-    </row>
-    <row r="10" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="37"/>
-    </row>
-    <row r="11" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="37"/>
-    </row>
-    <row r="12" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="63" t="s">
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="31"/>
+    </row>
+    <row r="13" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43">
+        <v>0</v>
+      </c>
+      <c r="B13" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="37"/>
-    </row>
-    <row r="13" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49">
-        <v>0</v>
-      </c>
-      <c r="B13" s="50" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="51" t="s">
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="31"/>
+    </row>
+    <row r="14" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="37"/>
-    </row>
-    <row r="14" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="B14" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="52" t="s">
+      <c r="H14" s="47"/>
+      <c r="I14" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54" t="s">
+      <c r="J14" s="77"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="31"/>
+    </row>
+    <row r="15" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="J14" s="67"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="37"/>
-    </row>
-    <row r="15" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="B15" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="72" t="s">
+      <c r="L15" s="31"/>
+    </row>
+    <row r="16" spans="1:12" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="L15" s="37"/>
-    </row>
-    <row r="16" spans="1:12" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
+      <c r="B16" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="C16" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="D16" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="E16" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="74"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="37"/>
+      <c r="F16" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="84"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="31"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2187,12 +2248,227 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB6B262-E400-4283-9FCD-D8097FCB10E4}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" style="33" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="33" customWidth="1"/>
+    <col min="3" max="6" width="16.33203125" style="33" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="51" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" style="51" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="51" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="33" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="33" customWidth="1"/>
+    <col min="12" max="12" width="1.77734375" style="33" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="33" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="31"/>
+    </row>
+    <row r="3" spans="1:12" ht="179.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+    </row>
+    <row r="4" spans="1:12" ht="310.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+    </row>
+    <row r="6" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="60"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="147"/>
+      <c r="K6" s="147"/>
+      <c r="L6" s="31"/>
+    </row>
+    <row r="7" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="60"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="148"/>
+      <c r="K7" s="148"/>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="8" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="60"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="149"/>
+      <c r="L8" s="31"/>
+    </row>
+    <row r="9" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="147"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="G9:J9"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF44DDF-8ED1-4864-8590-37C9E8A63962}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="150" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6DA28D-9BA1-40F8-AF7E-6A559A47F027}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2211,24 +2487,24 @@
       <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="26" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+    <row r="3" spans="1:4" s="20" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2240,17 +2516,278 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF44DDF-8ED1-4864-8590-37C9E8A63962}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBADC2D-2F39-4DD0-9F8C-1B88F9D121D3}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.21875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="31.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96"/>
+    </row>
+    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="164" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="166"/>
+    </row>
+    <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="164" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="166"/>
+    </row>
+    <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="167" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="168"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="169"/>
+    </row>
+    <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="170"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="170"/>
+      <c r="F5" s="171"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="153"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="155"/>
+    </row>
+    <row r="7" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="153"/>
+      <c r="C7" s="154"/>
+      <c r="D7" s="154"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="155"/>
+    </row>
+    <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="156" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="157"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="158"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="153"/>
+      <c r="C9" s="154"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="155"/>
+    </row>
+    <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="153"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154"/>
+      <c r="F10" s="155"/>
+    </row>
+    <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="153"/>
+      <c r="C11" s="154"/>
+      <c r="D11" s="154"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="155"/>
+    </row>
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="153"/>
+      <c r="C12" s="154"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="155"/>
+    </row>
+    <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="153"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="154"/>
+      <c r="F13" s="155"/>
+    </row>
+    <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="156" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="157"/>
+      <c r="C14" s="157"/>
+      <c r="D14" s="157"/>
+      <c r="E14" s="157"/>
+      <c r="F14" s="158"/>
+    </row>
+    <row r="15" spans="1:6" ht="140.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="159"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="161"/>
+    </row>
+    <row r="16" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="162" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="163"/>
+      <c r="D16" s="162" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="163"/>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="151"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="152"/>
+      <c r="F18" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="71" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Angsana New,Bold"&amp;12QMTS-SFR-24, Rev. 00, 17/08/22&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB07D9-A724-49B0-8EB6-7A0CF35A6E44}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="150" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2259,7 +2796,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2273,40 +2810,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="86"/>
+      <c r="A1" s="94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="96"/>
     </row>
     <row r="2" spans="1:15" ht="246.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="156"/>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="157"/>
-      <c r="K2" s="157"/>
-      <c r="L2" s="157"/>
-      <c r="M2" s="157"/>
-      <c r="N2" s="157"/>
-      <c r="O2" s="158"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2327,7 +2864,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2341,106 +2878,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="96"/>
+    </row>
+    <row r="2" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="86"/>
-    </row>
-    <row r="2" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="B2" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="C2" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="D2" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="89" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="91"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="104"/>
     </row>
     <row r="3" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="33" t="s">
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="F3" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="G3" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="H3" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="I3" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="J3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="K3" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="L3" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="M3" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="N3" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="O3" s="27" t="s">
         <v>92</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2480,37 +3017,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+    </row>
+    <row r="2" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-    </row>
-    <row r="2" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="159" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="159" t="s">
+      <c r="C2" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="159" t="s">
+      <c r="D2" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="159" t="s">
+      <c r="E2" s="53" t="s">
         <v>98</v>
-      </c>
-      <c r="E2" s="159" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="7"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2545,52 +3082,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="58" t="s">
+      <c r="C2" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="D2" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="E2" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="F2" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="G2" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="54" t="s">
         <v>105</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="160" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="7"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2606,87 +3143,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FFD366-79C9-44D9-ACB3-0A9172B78CCB}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="43.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="160" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="71" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"Angsana New,Bold"&amp;12QMTS-SFR-24, Rev. 00, 17/08/22&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
@@ -2706,14 +3166,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="107"/>
     </row>
     <row r="2" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2756,232 +3216,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBADC2D-2F39-4DD0-9F8C-1B88F9D121D3}">
-  <dimension ref="A1:F18"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FFD366-79C9-44D9-ACB3-0A9172B78CCB}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.21875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="31.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="145.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94"/>
-    </row>
-    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="110"/>
-    </row>
-    <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="110"/>
-    </row>
-    <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="111" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="113"/>
-    </row>
-    <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="114"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="114"/>
-      <c r="F5" s="115"/>
-    </row>
-    <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="99"/>
-    </row>
-    <row r="7" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="99"/>
-    </row>
-    <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="102"/>
-    </row>
-    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="97"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="99"/>
-    </row>
-    <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-    </row>
-    <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="97"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="99"/>
-    </row>
-    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="99"/>
-    </row>
-    <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="99"/>
-    </row>
-    <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="100" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="102"/>
-    </row>
-    <row r="15" spans="1:6" ht="140.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="103"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
-    </row>
-    <row r="16" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="106" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="107"/>
-      <c r="D16" s="106" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="107"/>
-      <c r="F16" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="95"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="32"/>
-    </row>
-    <row r="18" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="95"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="32"/>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="94" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="71" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Angsana New,Bold"&amp;12QMTS-SFR-24, Rev. 00, 17/08/22&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E915790A-876B-43BE-94E0-E24AD61D7CF9}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" customWidth="1"/>
+    <col min="4" max="15" width="7.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="96"/>
+    </row>
+    <row r="2" spans="1:15" ht="246.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="97" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="99"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2997,7 +3350,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3006,336 +3359,337 @@
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="4.5546875" style="27" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="27" customWidth="1"/>
+    <col min="6" max="8" width="4.5546875" style="21" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="21" customWidth="1"/>
     <col min="10" max="10" width="32.109375" style="1" customWidth="1"/>
-    <col min="11" max="13" width="4.5546875" style="27" customWidth="1"/>
-    <col min="14" max="14" width="33" style="27" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" style="27" customWidth="1"/>
+    <col min="11" max="13" width="4.5546875" style="21" customWidth="1"/>
+    <col min="14" max="14" width="33" style="21" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" style="21" customWidth="1"/>
     <col min="16" max="16" width="17.44140625" style="2" customWidth="1"/>
     <col min="17" max="17" width="9.109375" style="1" customWidth="1"/>
     <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-    </row>
-    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+    </row>
+    <row r="2" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="59"/>
+    </row>
+    <row r="3" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="153" t="s">
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="154"/>
-      <c r="O3" s="154"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="135" t="s">
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="145"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="146"/>
+      <c r="Q3" s="59"/>
+    </row>
+    <row r="4" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="136"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="137" t="s">
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="138"/>
-      <c r="M4" s="139"/>
-      <c r="N4" s="146"/>
-      <c r="O4" s="146"/>
-      <c r="P4" s="147"/>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="135"/>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="150"/>
-      <c r="O5" s="150"/>
-      <c r="P5" s="151"/>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="134" t="s">
+      <c r="L4" s="130"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="138"/>
+      <c r="O4" s="138"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="59"/>
+    </row>
+    <row r="5" spans="1:17" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="127"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="137"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="142"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="59"/>
+    </row>
+    <row r="6" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="137" t="s">
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="138"/>
-      <c r="M6" s="139"/>
-      <c r="N6" s="146"/>
-      <c r="O6" s="146"/>
-      <c r="P6" s="147"/>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="135"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="141"/>
-      <c r="M7" s="142"/>
-      <c r="N7" s="148"/>
-      <c r="O7" s="148"/>
-      <c r="P7" s="149"/>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="134" t="s">
+      <c r="L6" s="130"/>
+      <c r="M6" s="131"/>
+      <c r="N6" s="138"/>
+      <c r="O6" s="138"/>
+      <c r="P6" s="139"/>
+      <c r="Q6" s="59"/>
+    </row>
+    <row r="7" spans="1:17" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="127"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="134"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="140"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="59"/>
+    </row>
+    <row r="8" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="140"/>
-      <c r="L8" s="141"/>
-      <c r="M8" s="142"/>
-      <c r="N8" s="148"/>
-      <c r="O8" s="148"/>
-      <c r="P8" s="149"/>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="134"/>
-      <c r="B9" s="136"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
-      <c r="J9" s="136"/>
-      <c r="K9" s="143"/>
-      <c r="L9" s="144"/>
-      <c r="M9" s="145"/>
-      <c r="N9" s="150"/>
-      <c r="O9" s="150"/>
-      <c r="P9" s="151"/>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="132"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="134"/>
+      <c r="N8" s="140"/>
+      <c r="O8" s="140"/>
+      <c r="P8" s="141"/>
+      <c r="Q8" s="59"/>
+    </row>
+    <row r="9" spans="1:17" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="126"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="135"/>
+      <c r="L9" s="136"/>
+      <c r="M9" s="137"/>
+      <c r="N9" s="142"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="143"/>
+      <c r="Q9" s="59"/>
+    </row>
+    <row r="10" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="120"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="122"/>
-      <c r="K10" s="123" t="s">
+      <c r="B10" s="112"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="124"/>
-      <c r="M10" s="125"/>
-      <c r="N10" s="126"/>
-      <c r="O10" s="126"/>
-      <c r="P10" s="127"/>
-      <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="2"/>
+      <c r="L10" s="116"/>
+      <c r="M10" s="117"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="59"/>
+    </row>
+    <row r="11" spans="1:17" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="59"/>
     </row>
     <row r="12" spans="1:17" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="128" t="s">
+      <c r="C12" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="128" t="s">
+      <c r="D12" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="131" t="s">
+      <c r="F12" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="132"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="17" t="s">
+      <c r="G12" s="124"/>
+      <c r="H12" s="125"/>
+      <c r="I12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="128" t="s">
+      <c r="J12" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="129" t="s">
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="116" t="s">
+      <c r="O12" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="118" t="s">
+      <c r="P12" s="110" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="128"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="20" t="s">
+      <c r="A13" s="120"/>
+      <c r="B13" s="120"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="128"/>
-      <c r="K13" s="22" t="s">
+      <c r="J13" s="120"/>
+      <c r="K13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="N13" s="130"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="119"/>
-    </row>
-    <row r="14" spans="1:17" s="26" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
+      <c r="N13" s="122"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="111"/>
+    </row>
+    <row r="14" spans="1:17" s="20" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3386,257 +3740,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ActivityName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <RefID xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <ApprovalStatus xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Pending</ApprovalStatus>
-    <Workflow xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Finished</Workflow>
-    <LockBy xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LockBy>
-    <WorkflowHistory xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <RelatedTo xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <UserInfo>
-        <DisplayName>PTTDIGITAL-APP-Supaporn T</DisplayName>
-        <AccountId>25</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PTTDIGITAL-APP-Supitchaya</DisplayName>
-        <AccountId>1727</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>s-MossFarmAdmin</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TOP QMQS (Act.) (Anchalee)</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TOP QMQS-Chawlit</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TOP QMQS-Oranich</DisplayName>
-        <AccountId>2153</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TOP QMQS-PRTR-Pakphinya T.</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TOP QMQS-PRTR-Wanicha</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TOP QMTS (Sermsak)</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\zsupapornt</DisplayName>
-        <AccountId>25</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\zsupitchayas</DisplayName>
-        <AccountId>1727</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\s-mossfarmadmin</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\s-sp19adm</DisplayName>
-        <AccountId>2517</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\anchalee</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\chawlit</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\oranich</DisplayName>
-        <AccountId>2153</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\zpakphinya</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\wanicha</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\sermsak</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </RelatedTo>
-    <KnowledgeComments xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <LockDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <ApprovedDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <TaxCatchAll xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <Value>67</Value>
-    </TaxCatchAll>
-    <DocumentType xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Form</DocumentType>
-    <WFActions xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <Level1 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">S6.0 : Manage information, knowledge and system</Level1>
-    <Section xmlns="90971145-0e3f-401e-a533-b224f340d0bb">QMTS</Section>
-    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">00</_Revision>
-    <LinkToLaw xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LinkToLaw>
-    <RefURL xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <Action xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <Level2 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">S6.2 Maintain QSSHE excellence</Level2>
-    <Activity xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <AreaName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <UnitName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <DocumentCode xmlns="90971145-0e3f-401e-a533-b224f340d0bb">QMTS-SFR-24</DocumentCode>
-    <IssuedDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <RevisedDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb">2022-08-16T17:00:00+00:00</RevisedDate>
-    <ShareWithCompany xmlns="90971145-0e3f-401e-a533-b224f340d0bb">PTT</ShareWithCompany>
-    <ShareWithSpecificGroup xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </ShareWithSpecificGroup>
-    <IsActive1 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">true</IsActive1>
-    <AmendmentRecord xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <ApprovedBy xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </ApprovedBy>
-    <AssignTo xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\zsupapornt</DisplayName>
-        <AccountId>25</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\zsupitchayas</DisplayName>
-        <AccountId>1727</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\s-mossfarmadmin</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\s-sp19adm</DisplayName>
-        <AccountId>2517</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\anchalee</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\chawlit</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\oranich</DisplayName>
-        <AccountId>2153</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\zpakphinya</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\wanicha</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\sermsak</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </AssignTo>
-    <KnowledgeStatus xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Finished</KnowledgeStatus>
-    <Area xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <Unit xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <Department1 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">QMVP</Department1>
-    <System xmlns="90971145-0e3f-401e-a533-b224f340d0bb">TIS 18001</System>
-    <o3d8169c58294ff997d3d56a97d36e37 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">S6.2 Maintain QSSHE excellence</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c36b4e93-9fec-465c-a818-b3f2e1393b42</TermId>
-        </TermInfo>
-      </Terms>
-    </o3d8169c58294ff997d3d56a97d36e37>
-    <ShareWith xmlns="90971145-0e3f-401e-a533-b224f340d0bb">PTT Group</ShareWith>
-    <Owner xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
-      <UserInfo>
-        <DisplayName>i:0#.w|thaioilnt\sermsak</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Issued xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
-    <TechnicalDocument xmlns="90971145-0e3f-401e-a533-b224f340d0bb">true</TechnicalDocument>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ISO Document" ma:contentTypeID="0x01010086934EBC94246946B23F5DD9F27BF11F00B2FADA0FA4969F4D83190839948D67F5" ma:contentTypeVersion="51" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="fe874aa8cdea4475ac883b87bea1de2d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90971145-0e3f-401e-a533-b224f340d0bb" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="55f8bd73-a108-495f-bfbd-f04bb513be94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f645651e80efe6f1c815ba2641e5d38c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="90971145-0e3f-401e-a533-b224f340d0bb"/>
@@ -4227,34 +4330,258 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1BCF8DD-F64D-40E2-9E31-964B85018AAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93835A57-0014-4DA9-A2E8-6D1E26215A39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B36565D-48F5-4A14-839C-2DA862D8E795}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="90971145-0e3f-401e-a533-b224f340d0bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ActivityName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <RefID xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <ApprovalStatus xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Pending</ApprovalStatus>
+    <Workflow xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Finished</Workflow>
+    <LockBy xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LockBy>
+    <WorkflowHistory xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <RelatedTo xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <UserInfo>
+        <DisplayName>PTTDIGITAL-APP-Supaporn T</DisplayName>
+        <AccountId>25</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PTTDIGITAL-APP-Supitchaya</DisplayName>
+        <AccountId>1727</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>s-MossFarmAdmin</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TOP QMQS (Act.) (Anchalee)</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TOP QMQS-Chawlit</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TOP QMQS-Oranich</DisplayName>
+        <AccountId>2153</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TOP QMQS-PRTR-Pakphinya T.</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TOP QMQS-PRTR-Wanicha</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TOP QMTS (Sermsak)</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\zsupapornt</DisplayName>
+        <AccountId>25</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\zsupitchayas</DisplayName>
+        <AccountId>1727</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\s-mossfarmadmin</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\s-sp19adm</DisplayName>
+        <AccountId>2517</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\anchalee</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\chawlit</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\oranich</DisplayName>
+        <AccountId>2153</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\zpakphinya</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\wanicha</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\sermsak</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </RelatedTo>
+    <KnowledgeComments xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <LockDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <ApprovedDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <TaxCatchAll xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <Value>67</Value>
+    </TaxCatchAll>
+    <DocumentType xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Form</DocumentType>
+    <WFActions xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <Level1 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">S6.0 : Manage information, knowledge and system</Level1>
+    <Section xmlns="90971145-0e3f-401e-a533-b224f340d0bb">QMTS</Section>
+    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">00</_Revision>
+    <LinkToLaw xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LinkToLaw>
+    <RefURL xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <Action xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <Level2 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">S6.2 Maintain QSSHE excellence</Level2>
+    <Activity xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <AreaName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <UnitName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <DocumentCode xmlns="90971145-0e3f-401e-a533-b224f340d0bb">QMTS-SFR-24</DocumentCode>
+    <IssuedDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <RevisedDate xmlns="90971145-0e3f-401e-a533-b224f340d0bb">2022-08-16T17:00:00+00:00</RevisedDate>
+    <ShareWithCompany xmlns="90971145-0e3f-401e-a533-b224f340d0bb">PTT</ShareWithCompany>
+    <ShareWithSpecificGroup xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </ShareWithSpecificGroup>
+    <IsActive1 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">true</IsActive1>
+    <AmendmentRecord xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <ApprovedBy xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </ApprovedBy>
+    <AssignTo xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\zsupapornt</DisplayName>
+        <AccountId>25</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\zsupitchayas</DisplayName>
+        <AccountId>1727</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\s-mossfarmadmin</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\s-sp19adm</DisplayName>
+        <AccountId>2517</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\anchalee</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\chawlit</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\oranich</DisplayName>
+        <AccountId>2153</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\zpakphinya</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\wanicha</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\sermsak</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </AssignTo>
+    <KnowledgeStatus xmlns="90971145-0e3f-401e-a533-b224f340d0bb">Finished</KnowledgeStatus>
+    <Area xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <Unit xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <Department1 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">QMVP</Department1>
+    <System xmlns="90971145-0e3f-401e-a533-b224f340d0bb">TIS 18001</System>
+    <o3d8169c58294ff997d3d56a97d36e37 xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">S6.2 Maintain QSSHE excellence</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">c36b4e93-9fec-465c-a818-b3f2e1393b42</TermId>
+        </TermInfo>
+      </Terms>
+    </o3d8169c58294ff997d3d56a97d36e37>
+    <ShareWith xmlns="90971145-0e3f-401e-a533-b224f340d0bb">PTT Group</ShareWith>
+    <Owner xmlns="90971145-0e3f-401e-a533-b224f340d0bb">
+      <UserInfo>
+        <DisplayName>i:0#.w|thaioilnt\sermsak</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Issued xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
+    <TechnicalDocument xmlns="90971145-0e3f-401e-a533-b224f340d0bb">true</TechnicalDocument>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70866C74-89F7-4E96-902B-60E69D0AD1FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4272,4 +4599,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1BCF8DD-F64D-40E2-9E31-964B85018AAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93835A57-0014-4DA9-A2E8-6D1E26215A39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B36565D-48F5-4A14-839C-2DA862D8E795}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="90971145-0e3f-401e-a533-b224f340d0bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>